<commit_message>
Página Web y App Archivos
</commit_message>
<xml_diff>
--- a/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
+++ b/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">Tabulación!$A$1:$K$116</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Técnicas!$A$1:$K$116</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -223,9 +223,6 @@
     <t>Computador</t>
   </si>
   <si>
-    <t>Informe</t>
-  </si>
-  <si>
     <t>Escuchar la opinión del dueño y/o administrador para el desarrollo del proyecto</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>Alan Darién Prada Fierro</t>
+  </si>
+  <si>
+    <t>Resultados escritos</t>
   </si>
 </sst>
 </file>
@@ -1206,34 +1206,73 @@
     <xf numFmtId="14" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="4" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="4" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1255,87 +1294,48 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="4" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="4" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1371,7 +1371,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1425,7 +1425,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1479,7 +1479,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,7 +1533,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1587,7 +1587,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1641,7 +1641,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,7 +1695,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,7 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IV85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -2049,55 +2049,55 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="87"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="13" spans="1:11" ht="30">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="B15" s="2"/>
@@ -2108,56 +2108,56 @@
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
     </row>
     <row r="17" spans="1:16" ht="18">
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="1:16" ht="18">
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="1:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
     </row>
     <row r="20" spans="1:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A20" s="29"/>
       <c r="B20" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="53"/>
+      <c r="D20" s="93"/>
       <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
@@ -2167,13 +2167,13 @@
     </row>
     <row r="21" spans="1:16" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="69"/>
+      <c r="D21" s="74"/>
       <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
@@ -2183,9 +2183,9 @@
     </row>
     <row r="22" spans="1:16" ht="36.75" thickBot="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
@@ -2215,10 +2215,10 @@
       <c r="C26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="62" t="s">
+      <c r="D26" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="62"/>
+      <c r="E26" s="77"/>
       <c r="F26" s="16" t="s">
         <v>16</v>
       </c>
@@ -2230,10 +2230,10 @@
       <c r="C27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="63" t="s">
+      <c r="D27" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="63"/>
+      <c r="E27" s="78"/>
       <c r="F27" s="19" t="s">
         <v>51</v>
       </c>
@@ -2245,10 +2245,10 @@
       <c r="C28" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="64"/>
+      <c r="E28" s="79"/>
       <c r="F28" s="8" t="s">
         <v>46</v>
       </c>
@@ -2260,10 +2260,10 @@
       <c r="C29" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="64"/>
+      <c r="E29" s="79"/>
       <c r="F29" s="8" t="s">
         <v>45</v>
       </c>
@@ -2271,43 +2271,43 @@
     <row r="30" spans="1:16" ht="25.5" customHeight="1">
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="25.5" customHeight="1">
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="25.5" customHeight="1">
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:13" ht="25.5" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -2321,43 +2321,43 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="60" t="s">
+      <c r="B39" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
     </row>
     <row r="41" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
       <c r="J41" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B42" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
+      <c r="B42" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
     </row>
     <row r="43" spans="1:13" ht="25.5" customHeight="1">
       <c r="B43" s="25"/>
@@ -2674,6 +2674,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
@@ -2690,19 +2703,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -2715,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:IS39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:K4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2737,56 +2737,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A3" s="72"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.25">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
     </row>
     <row r="5" spans="1:10" s="45" customFormat="1" ht="20.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
     </row>
     <row r="6" spans="1:10" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1"/>
     <row r="8" spans="1:10" ht="15" thickBot="1">
@@ -2826,38 +2826,38 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="36" customFormat="1" ht="60" customHeight="1">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="76">
+      <c r="D10" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="51">
         <v>44967</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="I10" s="52" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="36" customFormat="1" ht="42" customHeight="1">
-      <c r="B11" s="71"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="46" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>61</v>
@@ -2876,17 +2876,17 @@
       </c>
     </row>
     <row r="12" spans="1:10" customFormat="1" ht="69.95" customHeight="1">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="94" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="46" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="49">
         <v>44974</v>
@@ -2902,15 +2902,15 @@
       </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" ht="60" customHeight="1">
-      <c r="B13" s="71"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="46" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="49">
         <v>44975</v>
@@ -2921,22 +2921,22 @@
       <c r="H13" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="53" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" customFormat="1" ht="43.5" customHeight="1">
-      <c r="B14" s="71" t="s">
-        <v>65</v>
+      <c r="B14" s="94" t="s">
+        <v>64</v>
       </c>
       <c r="C14" s="46" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="49">
         <v>44982</v>
@@ -2947,31 +2947,31 @@
       <c r="H14" s="49">
         <v>0</v>
       </c>
-      <c r="I14" s="78" t="s">
+      <c r="I14" s="53" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80" t="s">
+      <c r="B15" s="95"/>
+      <c r="C15" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="81" t="s">
+      <c r="D15" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="81">
+      <c r="F15" s="55">
         <v>44982</v>
       </c>
-      <c r="G15" s="81" t="s">
+      <c r="G15" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="81" t="s">
+      <c r="H15" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="I15" s="82" t="s">
+      <c r="I15" s="56" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3174,60 +3174,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="12" spans="1:11">
@@ -3437,60 +3437,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -3503,17 +3503,17 @@
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1">
       <c r="A15" s="29"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="90" t="s">
+      <c r="B15" s="57"/>
+      <c r="C15" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="E15" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="92" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="85"/>
+      <c r="F15" s="59"/>
       <c r="G15" s="24"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -3521,17 +3521,17 @@
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A16" s="29"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="89">
+      <c r="B16" s="58"/>
+      <c r="C16" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="63">
         <v>44967</v>
       </c>
-      <c r="E16" s="96" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="86"/>
+      <c r="E16" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="60"/>
       <c r="G16" s="24"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -3539,15 +3539,15 @@
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="80.099999999999994" customHeight="1">
       <c r="A17" s="29"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="87">
+      <c r="B17" s="57"/>
+      <c r="C17" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="61">
         <v>44968</v>
       </c>
-      <c r="E17" s="97" t="s">
-        <v>82</v>
+      <c r="E17" s="71" t="s">
+        <v>81</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="24"/>
@@ -3557,15 +3557,15 @@
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="90" customHeight="1">
       <c r="A18" s="29"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="87">
+      <c r="B18" s="58"/>
+      <c r="C18" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="61">
         <v>44974</v>
       </c>
-      <c r="E18" s="97" t="s">
-        <v>83</v>
+      <c r="E18" s="71" t="s">
+        <v>82</v>
       </c>
       <c r="F18" s="34"/>
       <c r="K18" s="13"/>
@@ -3574,42 +3574,42 @@
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="90" customHeight="1">
       <c r="A19" s="29"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="87">
+      <c r="B19" s="57"/>
+      <c r="C19" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="61">
         <v>44975</v>
       </c>
-      <c r="E19" s="97" t="s">
-        <v>85</v>
+      <c r="E19" s="71" t="s">
+        <v>84</v>
       </c>
       <c r="F19" s="34"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="69.95" customHeight="1">
       <c r="A20" s="29"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="94" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="87">
+      <c r="B20" s="58"/>
+      <c r="C20" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="61">
         <v>44983</v>
       </c>
-      <c r="E20" s="97"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="34"/>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="69.95" customHeight="1" thickBot="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="95" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="88">
+      <c r="B21" s="57"/>
+      <c r="C21" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="62">
         <v>44983</v>
       </c>
-      <c r="E21" s="98"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="34"/>
       <c r="IW21" s="2"/>
     </row>
@@ -3787,60 +3787,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4083,60 +4083,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4396,56 +4396,56 @@
       <c r="IV4" s="1"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
       <c r="IV5" s="1"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
       <c r="IT6" s="1"/>
       <c r="IU6" s="1"/>
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="30">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="57"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
       <c r="IT7" s="1"/>
       <c r="IU7" s="1"/>
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="30">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
       <c r="IV8" s="1"/>
@@ -4456,17 +4456,17 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="1:256" ht="15" thickTop="1">
       <c r="IT11" s="1"/>

</xml_diff>

<commit_message>
Plan Proyecto y Diagramas UML
</commit_message>
<xml_diff>
--- a/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
+++ b/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
@@ -202,9 +202,6 @@
     <t>Conocer cómo funciona la empresa o negocio - administración</t>
   </si>
   <si>
-    <t>Medir la percepción de los clientes al recibir su producto y su nivel de satisfacción al consumirlo</t>
-  </si>
-  <si>
     <t>Tienda la Antioqueño</t>
   </si>
   <si>
@@ -263,6 +260,9 @@
   </si>
   <si>
     <t>Alan Darién Prada Fierro</t>
+  </si>
+  <si>
+    <t>Percibir el punto de vista y opinión de el dueño o administrador acerca del proyecto a realizar</t>
   </si>
 </sst>
 </file>
@@ -1232,36 +1232,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1283,15 +1255,43 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1301,16 +1301,16 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="17" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1350,7 +1350,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,7 +1404,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1458,7 +1458,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1512,7 +1512,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1566,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1620,7 +1620,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,7 +1674,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2028,55 +2028,55 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="73"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="73"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="13" spans="1:11" ht="30">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="B15" s="2"/>
@@ -2087,56 +2087,56 @@
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
     </row>
     <row r="17" spans="1:16" ht="18">
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
     </row>
     <row r="18" spans="1:16" ht="18">
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
     </row>
     <row r="19" spans="1:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
     </row>
     <row r="20" spans="1:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A20" s="29"/>
       <c r="B20" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="79"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="21" spans="1:16" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="69"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
@@ -2162,9 +2162,9 @@
     </row>
     <row r="22" spans="1:16" ht="36.75" thickBot="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
@@ -2194,10 +2194,10 @@
       <c r="C26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="83"/>
+      <c r="E26" s="73"/>
       <c r="F26" s="16" t="s">
         <v>16</v>
       </c>
@@ -2209,10 +2209,10 @@
       <c r="C27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="84"/>
+      <c r="E27" s="74"/>
       <c r="F27" s="19" t="s">
         <v>48</v>
       </c>
@@ -2224,10 +2224,10 @@
       <c r="C28" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="85" t="s">
+      <c r="D28" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="85"/>
+      <c r="E28" s="75"/>
       <c r="F28" s="8" t="s">
         <v>43</v>
       </c>
@@ -2239,10 +2239,10 @@
       <c r="C29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="85"/>
+      <c r="E29" s="75"/>
       <c r="F29" s="8" t="s">
         <v>42</v>
       </c>
@@ -2250,43 +2250,43 @@
     <row r="30" spans="1:16" ht="25.5" customHeight="1">
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="25.5" customHeight="1">
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="25.5" customHeight="1">
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:13" ht="25.5" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -2300,43 +2300,43 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="81" t="s">
+      <c r="B39" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="80"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
     </row>
     <row r="41" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="80"/>
-      <c r="F41" s="80"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
       <c r="J41" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B42" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
+      <c r="B42" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
     </row>
     <row r="43" spans="1:13" ht="25.5" customHeight="1">
       <c r="B43" s="25"/>
@@ -2653,6 +2653,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
@@ -2669,19 +2682,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -2695,7 +2695,7 @@
   <dimension ref="A3:IS39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2756,16 +2756,16 @@
       <c r="J5" s="94"/>
     </row>
     <row r="6" spans="1:10" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1"/>
     <row r="8" spans="1:10" ht="15" thickBot="1">
@@ -2805,17 +2805,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="36" customFormat="1" ht="60" customHeight="1">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="90" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="51">
         <v>44967</v>
@@ -2824,22 +2824,22 @@
         <v>50</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I10" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="36" customFormat="1" ht="42" customHeight="1">
-      <c r="B11" s="90"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="46" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="49">
         <v>44968</v>
@@ -2855,39 +2855,39 @@
       </c>
     </row>
     <row r="12" spans="1:10" customFormat="1" ht="69.95" customHeight="1">
-      <c r="B12" s="90" t="s">
-        <v>57</v>
+      <c r="B12" s="91" t="s">
+        <v>77</v>
       </c>
       <c r="C12" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="96" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="96">
+        <v>38</v>
+      </c>
+      <c r="D12" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="97">
         <v>44975</v>
       </c>
-      <c r="G12" s="96" t="s">
+      <c r="G12" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="97" t="s">
+      <c r="H12" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="99" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="B13" s="91"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
       <c r="I13" s="100"/>
     </row>
     <row r="14" spans="1:10" customFormat="1" ht="43.5" customHeight="1">
@@ -3107,60 +3107,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="12" spans="1:11">
@@ -3370,60 +3370,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -3438,13 +3438,13 @@
       <c r="A15" s="29"/>
       <c r="B15" s="53"/>
       <c r="C15" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="E15" s="62" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="55"/>
       <c r="G15" s="24"/>
@@ -3456,13 +3456,13 @@
       <c r="A16" s="29"/>
       <c r="B16" s="54"/>
       <c r="C16" s="63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="59">
         <v>44967</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="24"/>
@@ -3474,13 +3474,13 @@
       <c r="A17" s="29"/>
       <c r="B17" s="53"/>
       <c r="C17" s="64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="57">
         <v>44968</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="24"/>
@@ -3492,13 +3492,13 @@
       <c r="A18" s="29"/>
       <c r="B18" s="54"/>
       <c r="C18" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="57">
         <v>44974</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="34"/>
       <c r="K18" s="13"/>
@@ -3509,13 +3509,13 @@
       <c r="A19" s="29"/>
       <c r="B19" s="53"/>
       <c r="C19" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="57">
         <v>44975</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="34"/>
       <c r="IW19" s="2"/>
@@ -3524,7 +3524,7 @@
       <c r="A20" s="29"/>
       <c r="B20" s="54"/>
       <c r="C20" s="64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="57">
         <v>44983</v>
@@ -3537,7 +3537,7 @@
       <c r="A21" s="29"/>
       <c r="B21" s="53"/>
       <c r="C21" s="65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="58">
         <v>44983</v>
@@ -3720,60 +3720,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4016,60 +4016,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4329,56 +4329,56 @@
       <c r="IV4" s="1"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
       <c r="IV5" s="1"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
       <c r="IT6" s="1"/>
       <c r="IU6" s="1"/>
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
       <c r="IT7" s="1"/>
       <c r="IU7" s="1"/>
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="30">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
       <c r="IV8" s="1"/>
@@ -4389,17 +4389,17 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" spans="1:256" ht="15" thickTop="1">
       <c r="IT11" s="1"/>

</xml_diff>

<commit_message>
Act. Hoja Control Cambios
</commit_message>
<xml_diff>
--- a/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
+++ b/docs/trim1/gestion_proyecto/1_recoleccion_informacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
   <si>
     <t>HOJA DE CONTROL</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>02/03/23</t>
+  </si>
+  <si>
+    <t>0.5.1</t>
+  </si>
+  <si>
+    <t>Renovación ("Tienda_Antio-Market_(web)\CLIENTE - COMPRADOR/ index.html"</t>
+  </si>
+  <si>
+    <t>03/03/23</t>
   </si>
 </sst>
 </file>
@@ -1250,8 +1259,36 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1271,34 +1308,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1368,7 +1377,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1431,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1476,7 +1485,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1530,7 +1539,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1584,7 +1593,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1647,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1692,7 +1701,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2020,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IV85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2046,55 +2055,55 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="13" spans="1:11" ht="30">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="B15" s="2"/>
@@ -2105,56 +2114,56 @@
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:16" ht="18">
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
     </row>
     <row r="18" spans="1:16" ht="18">
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
     </row>
     <row r="19" spans="1:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
     </row>
     <row r="20" spans="1:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A20" s="29"/>
       <c r="B20" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="89" t="s">
+      <c r="C20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="89"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
@@ -2164,13 +2173,13 @@
     </row>
     <row r="21" spans="1:16" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="70"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
@@ -2180,9 +2189,9 @@
     </row>
     <row r="22" spans="1:16" ht="36.75" thickBot="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="79"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
@@ -2212,10 +2221,10 @@
       <c r="C26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="73"/>
+      <c r="E26" s="83"/>
       <c r="F26" s="16" t="s">
         <v>16</v>
       </c>
@@ -2227,10 +2236,10 @@
       <c r="C27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="74"/>
+      <c r="E27" s="84"/>
       <c r="F27" s="19" t="s">
         <v>48</v>
       </c>
@@ -2242,10 +2251,10 @@
       <c r="C28" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="75"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="8" t="s">
         <v>43</v>
       </c>
@@ -2257,10 +2266,10 @@
       <c r="C29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="75"/>
+      <c r="E29" s="85"/>
       <c r="F29" s="8" t="s">
         <v>42</v>
       </c>
@@ -2272,10 +2281,10 @@
       <c r="C30" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="75"/>
+      <c r="E30" s="85"/>
       <c r="F30" s="8" t="s">
         <v>80</v>
       </c>
@@ -2287,40 +2296,48 @@
       <c r="C31" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="75" t="s">
+      <c r="D31" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="75"/>
+      <c r="E31" s="85"/>
       <c r="F31" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="25.5" customHeight="1">
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="8"/>
+    <row r="32" spans="1:16" ht="80.099999999999994" customHeight="1">
+      <c r="B32" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="85"/>
+      <c r="F32" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="25.5" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -2334,43 +2351,43 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B40" s="69" t="s">
+      <c r="B40" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
     </row>
     <row r="41" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="80"/>
+      <c r="F41" s="80"/>
       <c r="J41" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
     </row>
     <row r="43" spans="1:13" ht="25.5" customHeight="1">
       <c r="B43" s="25"/>
@@ -2687,19 +2704,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:D20"/>
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
@@ -2716,6 +2720,19 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -2790,16 +2807,16 @@
       <c r="J5" s="94"/>
     </row>
     <row r="6" spans="1:10" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1"/>
     <row r="8" spans="1:10" ht="15" thickBot="1">
@@ -3141,60 +3158,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="10" spans="1:11" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="12" spans="1:11">
@@ -3380,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3404,60 +3421,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -3754,60 +3771,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4050,60 +4067,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="10" spans="1:257" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -4363,56 +4380,56 @@
       <c r="IV4" s="1"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
       <c r="IV5" s="1"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
       <c r="IT6" s="1"/>
       <c r="IU6" s="1"/>
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="30">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
       <c r="IT7" s="1"/>
       <c r="IU7" s="1"/>
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="30">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
       <c r="IV8" s="1"/>
@@ -4423,17 +4440,17 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" s="44" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:256" ht="15" thickTop="1">
       <c r="IT11" s="1"/>

</xml_diff>